<commit_message>
re-structure project and docs generation
</commit_message>
<xml_diff>
--- a/docs/dwworksheet/High_Level_Dimensional_Modeling_Workbook.xlsx
+++ b/docs/dwworksheet/High_Level_Dimensional_Modeling_Workbook.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6ff47dbd60957bc3/Desktop/remitproworkstation/data-warehouse-poc/docs/dwworksheet/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6ff47dbd60957bc3/Desktop/remitproworkstation/data-warehouse/docs/dwworksheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="25" documentId="11_EE58D9C42079E042CC2ADDA3843172BBE23BFBFF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4D2A2470-0EE9-4122-9150-12F5F0688A95}"/>
+  <xr:revisionPtr revIDLastSave="58" documentId="11_EE58D9C42079E042CC2ADDA3843172BBE23BFBFF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{01796DA5-99AD-4638-939D-5362BD7B92F7}"/>
   <bookViews>
-    <workbookView xWindow="216" yWindow="552" windowWidth="21600" windowHeight="11232" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="216" yWindow="264" windowWidth="16224" windowHeight="11520" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Readme" sheetId="5" r:id="rId1"/>
@@ -577,7 +577,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="56">
   <si>
     <t>Description</t>
   </si>
@@ -600,27 +600,6 @@
     <t>Fact
 Grain
 Type</t>
-  </si>
-  <si>
-    <t>Dim8</t>
-  </si>
-  <si>
-    <t>Dim9</t>
-  </si>
-  <si>
-    <t>Dim10</t>
-  </si>
-  <si>
-    <t>Dim11</t>
-  </si>
-  <si>
-    <t>Dim12</t>
-  </si>
-  <si>
-    <t>Dim13</t>
-  </si>
-  <si>
-    <t>Dim14</t>
   </si>
   <si>
     <t>Instructions!</t>
@@ -680,47 +659,113 @@
     <t>DimCustomer</t>
   </si>
   <si>
-    <t>DimPromosion</t>
-  </si>
-  <si>
-    <t>DimCurrency</t>
-  </si>
-  <si>
-    <t>DimSalesTerrytory</t>
-  </si>
-  <si>
-    <t>FactInternetSales</t>
-  </si>
-  <si>
     <t>x</t>
-  </si>
-  <si>
-    <t>FactInternetSalesReason</t>
-  </si>
-  <si>
-    <t>DimSalesReason</t>
-  </si>
-  <si>
-    <t>FactProductInventory</t>
   </si>
   <si>
     <t>DimProduct</t>
   </si>
   <si>
-    <t>Internet Sales</t>
+    <t>DimEmployee</t>
   </si>
   <si>
-    <t xml:space="preserve">Internet Sales Reason </t>
+    <t>Sales</t>
   </si>
   <si>
-    <t xml:space="preserve">Product Inventory </t>
+    <t>FactSales</t>
+  </si>
+  <si>
+    <t>CustomerID</t>
+  </si>
+  <si>
+    <t>CompanyName</t>
+  </si>
+  <si>
+    <t>ContactName</t>
+  </si>
+  <si>
+    <t>ContactTitle</t>
+  </si>
+  <si>
+    <t>CustomerCountry</t>
+  </si>
+  <si>
+    <t>CustomerRegion</t>
+  </si>
+  <si>
+    <t>CustomerCity</t>
+  </si>
+  <si>
+    <t>CustomerPostalCode</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>FullDateUSA</t>
+  </si>
+  <si>
+    <t>DayOfWeek</t>
+  </si>
+  <si>
+    <t>DayName</t>
+  </si>
+  <si>
+    <t>DayOfMonth</t>
+  </si>
+  <si>
+    <t>DayOfYear</t>
+  </si>
+  <si>
+    <t>WeekOfYear</t>
+  </si>
+  <si>
+    <t>MonthName</t>
+  </si>
+  <si>
+    <t>MonthOfYear</t>
+  </si>
+  <si>
+    <t>Quarter</t>
+  </si>
+  <si>
+    <t>QuarterName</t>
+  </si>
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>IsWeekday</t>
+  </si>
+  <si>
+    <t>ProductID</t>
+  </si>
+  <si>
+    <t>ProductName</t>
+  </si>
+  <si>
+    <t>Discontinued</t>
+  </si>
+  <si>
+    <t>SupplierName</t>
+  </si>
+  <si>
+    <t>CategoryName</t>
+  </si>
+  <si>
+    <t>EmployeeID</t>
+  </si>
+  <si>
+    <t>EmployeeName</t>
+  </si>
+  <si>
+    <t>EmployeeTitle</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -757,6 +802,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -818,7 +868,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -847,6 +897,12 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1616,11 +1672,11 @@
   </sheetPr>
   <dimension ref="A1:S23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B12" sqref="B12"/>
+      <selection pane="bottomRight" activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1636,7 +1692,7 @@
   <sheetData>
     <row r="1" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:19" ht="66.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -1656,72 +1712,52 @@
         <v>2</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="J2" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="K2" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="L2" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="M2" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="N2" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="O2" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="P2" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q2" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="R2" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="S2" s="6" t="s">
-        <v>12</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6"/>
+      <c r="L2" s="6"/>
+      <c r="M2" s="6"/>
+      <c r="N2" s="6"/>
+      <c r="O2" s="6"/>
+      <c r="P2" s="6"/>
+      <c r="Q2" s="6"/>
+      <c r="R2" s="6"/>
+      <c r="S2" s="6"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
       <c r="F3" s="4" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="K3" s="4"/>
       <c r="L3" s="4"/>
@@ -1734,12 +1770,8 @@
       <c r="S3" s="4"/>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A4" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>34</v>
-      </c>
+      <c r="A4" s="5"/>
+      <c r="B4" s="3"/>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
@@ -1748,9 +1780,7 @@
       <c r="H4" s="4"/>
       <c r="I4" s="4"/>
       <c r="J4" s="4"/>
-      <c r="K4" s="4" t="s">
-        <v>33</v>
-      </c>
+      <c r="K4" s="4"/>
       <c r="L4" s="4"/>
       <c r="M4" s="4"/>
       <c r="N4" s="4"/>
@@ -1761,26 +1791,18 @@
       <c r="S4" s="4"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A5" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>36</v>
-      </c>
+      <c r="A5" s="5"/>
+      <c r="B5" s="3"/>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
-      <c r="F5" s="4" t="s">
-        <v>33</v>
-      </c>
+      <c r="F5" s="4"/>
       <c r="G5" s="4"/>
       <c r="H5" s="4"/>
       <c r="I5" s="4"/>
       <c r="J5" s="4"/>
       <c r="K5" s="4"/>
-      <c r="L5" s="4" t="s">
-        <v>33</v>
-      </c>
+      <c r="L5" s="4"/>
       <c r="M5" s="4"/>
       <c r="N5" s="4"/>
       <c r="O5" s="4"/>
@@ -2181,9 +2203,9 @@
   </sheetPr>
   <dimension ref="A1:E64"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3:B12"/>
+      <selection pane="bottomLeft" activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2198,227 +2220,291 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="13" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="C2" s="12" t="s">
         <v>0</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="B3" s="3"/>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
+      <c r="B4" s="15" t="s">
+        <v>28</v>
+      </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
+      <c r="B5" s="15" t="s">
+        <v>29</v>
+      </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
+      <c r="B6" s="15" t="s">
+        <v>30</v>
+      </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
+      <c r="B7" s="15" t="s">
+        <v>31</v>
+      </c>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
+      <c r="B8" s="15" t="s">
+        <v>32</v>
+      </c>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
+      <c r="B9" s="15" t="s">
+        <v>33</v>
+      </c>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
+      <c r="B10" s="15" t="s">
+        <v>34</v>
+      </c>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="3"/>
-      <c r="B11" s="3"/>
+      <c r="A11" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="15" t="s">
+        <v>35</v>
+      </c>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="3"/>
-      <c r="B12" s="3"/>
+      <c r="B12" s="16" t="s">
+        <v>36</v>
+      </c>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="3"/>
-      <c r="B13" s="3"/>
+      <c r="B13" s="15" t="s">
+        <v>37</v>
+      </c>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="3"/>
-      <c r="B14" s="3"/>
+      <c r="B14" s="15" t="s">
+        <v>38</v>
+      </c>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="3"/>
-      <c r="B15" s="3"/>
+      <c r="B15" s="15" t="s">
+        <v>39</v>
+      </c>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="3"/>
-      <c r="B16" s="3"/>
+      <c r="B16" s="15" t="s">
+        <v>40</v>
+      </c>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="3"/>
-      <c r="B17" s="3"/>
+      <c r="B17" s="15" t="s">
+        <v>41</v>
+      </c>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="3"/>
-      <c r="B18" s="3"/>
+      <c r="B18" s="15" t="s">
+        <v>42</v>
+      </c>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="3"/>
-      <c r="B19" s="3"/>
+      <c r="B19" s="15" t="s">
+        <v>43</v>
+      </c>
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="3"/>
-      <c r="B20" s="3"/>
+      <c r="B20" s="15" t="s">
+        <v>44</v>
+      </c>
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
       <c r="E20" s="3"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="3"/>
-      <c r="B21" s="3"/>
+      <c r="B21" s="15" t="s">
+        <v>45</v>
+      </c>
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
       <c r="E21" s="3"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="3"/>
-      <c r="B22" s="3"/>
+      <c r="B22" s="15" t="s">
+        <v>46</v>
+      </c>
       <c r="C22" s="3"/>
       <c r="D22" s="3"/>
       <c r="E22" s="3"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="3"/>
-      <c r="B23" s="3"/>
+      <c r="B23" s="15" t="s">
+        <v>47</v>
+      </c>
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
       <c r="E23" s="3"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A24" s="3"/>
-      <c r="B24" s="3"/>
+      <c r="A24" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B24" s="15" t="s">
+        <v>48</v>
+      </c>
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="3"/>
-      <c r="B25" s="3"/>
+      <c r="B25" s="15" t="s">
+        <v>49</v>
+      </c>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="3"/>
-      <c r="B26" s="3"/>
+      <c r="B26" s="15" t="s">
+        <v>50</v>
+      </c>
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
       <c r="E26" s="3"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="3"/>
-      <c r="B27" s="3"/>
+      <c r="B27" s="15" t="s">
+        <v>51</v>
+      </c>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
       <c r="E27" s="3"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="3"/>
-      <c r="B28" s="3"/>
+      <c r="B28" s="15" t="s">
+        <v>52</v>
+      </c>
       <c r="C28" s="3"/>
       <c r="D28" s="3"/>
       <c r="E28" s="3"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A29" s="3"/>
-      <c r="B29" s="3"/>
+      <c r="A29" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B29" s="15" t="s">
+        <v>53</v>
+      </c>
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
       <c r="E29" s="3"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="3"/>
-      <c r="B30" s="3"/>
+      <c r="B30" s="15" t="s">
+        <v>54</v>
+      </c>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
       <c r="E30" s="3"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="3"/>
-      <c r="B31" s="3"/>
+      <c r="B31" s="15" t="s">
+        <v>55</v>
+      </c>
       <c r="C31" s="3"/>
       <c r="D31" s="3"/>
       <c r="E31" s="3"/>
@@ -2688,31 +2774,31 @@
   <sheetData>
     <row r="1" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="C1" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="D1" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="E1" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="F1" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="G1" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="H1" s="10" t="s">
-        <v>21</v>
-      </c>
       <c r="I1" s="10" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">

</xml_diff>